<commit_message>
Add young interference data
</commit_message>
<xml_diff>
--- a/LO6/IY/data/data.xlsx
+++ b/LO6/IY/data/data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinplanck/Desktop/Physics/Physics Lab III/LO6/IY/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{322104F6-2DFE-6E4E-8270-0D7C7D4198CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30BDDFC-8CD5-7945-A597-30F1E7BD6903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{FDF36B51-70B8-0C4B-B0D3-FEA7D65BAA04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D194B9-A3C8-0A48-B727-4088EFFD3ED9}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="113" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>